<commit_message>
match the database naming with the python code
</commit_message>
<xml_diff>
--- a/src/databases/Equipment_Database_python.xlsx
+++ b/src/databases/Equipment_Database_python.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="hammer" sheetId="28" r:id="rId1"/>
     <sheet name="drilling rig" sheetId="29" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcMode="autoNoTable" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -38,9 +38,6 @@
     <t>hammer with sleeve lenght</t>
   </si>
   <si>
-    <t>pile sleeve diameter</t>
-  </si>
-  <si>
     <t>total weight</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>name (-)</t>
+  </si>
+  <si>
+    <t>Sleeve diameter [m]</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,61 +639,61 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -756,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,91 +765,91 @@
     <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Z1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AB1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ongoing debug of v_select.py
</commit_message>
<xml_diff>
--- a/src/databases/Equipment_Database_python.xlsx
+++ b/src/databases/Equipment_Database_python.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7160"/>
   </bookViews>
   <sheets>
     <sheet name="hammer" sheetId="28" r:id="rId1"/>
@@ -596,33 +596,33 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="10" max="10" width="14.7265625" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" customWidth="1"/>
+    <col min="18" max="18" width="13.81640625" customWidth="1"/>
     <col min="19" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.42578125" customWidth="1"/>
-    <col min="24" max="24" width="11.85546875" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="14.7265625" customWidth="1"/>
+    <col min="22" max="22" width="12.453125" customWidth="1"/>
+    <col min="24" max="24" width="11.81640625" customWidth="1"/>
+    <col min="25" max="25" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
@@ -696,7 +696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -760,9 +760,9 @@
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>53</v>
@@ -852,7 +852,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
many changes - main and selection working
</commit_message>
<xml_diff>
--- a/src/databases/Equipment_Database_python.xlsx
+++ b/src/databases/Equipment_Database_python.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hammer" sheetId="28" r:id="rId1"/>
-    <sheet name="drilling rig" sheetId="29" r:id="rId2"/>
+    <sheet name="drill rig" sheetId="29" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="autoNoTable" calcOnSave="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -595,34 +595,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
-    <col min="10" max="10" width="14.7265625" customWidth="1"/>
-    <col min="11" max="11" width="16.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13.26953125" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" customWidth="1"/>
-    <col min="15" max="15" width="15.81640625" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" customWidth="1"/>
-    <col min="18" max="18" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1"/>
     <col min="19" max="20" width="11" customWidth="1"/>
-    <col min="21" max="21" width="14.7265625" customWidth="1"/>
-    <col min="22" max="22" width="12.453125" customWidth="1"/>
-    <col min="24" max="24" width="11.81640625" customWidth="1"/>
-    <col min="25" max="25" width="11.54296875" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
@@ -696,7 +696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -756,13 +756,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>53</v>
@@ -852,7 +852,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>

</xml_diff>